<commit_message>
added conclusion about the API
</commit_message>
<xml_diff>
--- a/_memoria/05_API Deep dive/familySearchParas.xlsx
+++ b/_memoria/05_API Deep dive/familySearchParas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" firstSheet="17" activeTab="28"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -13,36 +13,37 @@
     <sheet name="FamilyView" sheetId="29" r:id="rId4"/>
     <sheet name="fact" sheetId="5" r:id="rId5"/>
     <sheet name="placeReference" sheetId="28" r:id="rId6"/>
-    <sheet name="user" sheetId="8" r:id="rId7"/>
-    <sheet name="relationship" sheetId="18" r:id="rId8"/>
-    <sheet name="childParentsRelationship" sheetId="19" r:id="rId9"/>
-    <sheet name="note" sheetId="17" r:id="rId10"/>
-    <sheet name="name" sheetId="9" r:id="rId11"/>
-    <sheet name="nameForm" sheetId="11" r:id="rId12"/>
-    <sheet name="namePart" sheetId="27" r:id="rId13"/>
-    <sheet name="date" sheetId="10" r:id="rId14"/>
-    <sheet name="ResourceReference" sheetId="13" r:id="rId15"/>
-    <sheet name="SourceDescription" sheetId="15" r:id="rId16"/>
-    <sheet name="SourceReference" sheetId="14" r:id="rId17"/>
-    <sheet name="SourceCitation" sheetId="16" r:id="rId18"/>
-    <sheet name="subject" sheetId="6" r:id="rId19"/>
-    <sheet name="conclusion" sheetId="7" r:id="rId20"/>
-    <sheet name="Collection" sheetId="21" r:id="rId21"/>
-    <sheet name="CollectionContent" sheetId="23" r:id="rId22"/>
-    <sheet name="Attribution" sheetId="20" r:id="rId23"/>
-    <sheet name="discussion" sheetId="30" r:id="rId24"/>
-    <sheet name="discussionReference" sheetId="31" r:id="rId25"/>
-    <sheet name="comment" sheetId="32" r:id="rId26"/>
-    <sheet name="link" sheetId="33" r:id="rId27"/>
-    <sheet name="changeInfo" sheetId="34" r:id="rId28"/>
-    <sheet name="changeInfo (2)" sheetId="35" r:id="rId29"/>
+    <sheet name="placeDescription" sheetId="36" r:id="rId7"/>
+    <sheet name="user" sheetId="8" r:id="rId8"/>
+    <sheet name="relationship" sheetId="18" r:id="rId9"/>
+    <sheet name="childParentsRelationship" sheetId="19" r:id="rId10"/>
+    <sheet name="note" sheetId="17" r:id="rId11"/>
+    <sheet name="name" sheetId="9" r:id="rId12"/>
+    <sheet name="nameForm" sheetId="11" r:id="rId13"/>
+    <sheet name="namePart" sheetId="27" r:id="rId14"/>
+    <sheet name="date" sheetId="10" r:id="rId15"/>
+    <sheet name="ResourceReference" sheetId="13" r:id="rId16"/>
+    <sheet name="SourceDescription" sheetId="15" r:id="rId17"/>
+    <sheet name="SourceReference" sheetId="14" r:id="rId18"/>
+    <sheet name="SourceCitation" sheetId="16" r:id="rId19"/>
+    <sheet name="subject" sheetId="6" r:id="rId20"/>
+    <sheet name="conclusion" sheetId="7" r:id="rId21"/>
+    <sheet name="Collection" sheetId="21" r:id="rId22"/>
+    <sheet name="CollectionContent" sheetId="23" r:id="rId23"/>
+    <sheet name="Attribution" sheetId="20" r:id="rId24"/>
+    <sheet name="discussion" sheetId="30" r:id="rId25"/>
+    <sheet name="discussionReference" sheetId="31" r:id="rId26"/>
+    <sheet name="comment" sheetId="32" r:id="rId27"/>
+    <sheet name="link" sheetId="33" r:id="rId28"/>
+    <sheet name="changeInfo" sheetId="34" r:id="rId29"/>
+    <sheet name="changeInfo (2)" sheetId="35" r:id="rId30"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="410">
   <si>
     <t>type</t>
   </si>
@@ -1224,6 +1225,54 @@
   </si>
   <si>
     <t>Els números de telèfon que pertanyen al individu o col·lectiu.</t>
+  </si>
+  <si>
+    <t>[placeDescription]</t>
+  </si>
+  <si>
+    <t>temporalDescription</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>spatialDescription</t>
+  </si>
+  <si>
+    <t>jurisdiction</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>[PlaceDisplayProperties]</t>
+  </si>
+  <si>
+    <t>Identificador que expressa el nivell de introduït de la localització. Per exemple, adreça, província, estat, pais, etcètera.</t>
+  </si>
+  <si>
+    <t>Una llista ordenada de valors estanderitzats o noramlitzats que descriuen la localització.</t>
+  </si>
+  <si>
+    <t>Descripció del moment tempora al que aquest nom aplica per la localització.</t>
+  </si>
+  <si>
+    <t>Desvació cap al nord o sur respecte l'equador.</t>
+  </si>
+  <si>
+    <t>Desviació cap al oest o est respecte l'queador.</t>
+  </si>
+  <si>
+    <t>Referència a la descripció geoespacial de la localització.</t>
+  </si>
+  <si>
+    <t>Referencia a la localització a la que es fa referència.</t>
+  </si>
+  <si>
+    <t>Propietats de visualització. Conté paràmetres en foramt string per pintar el nom complet de la localització, el nom curt i el 'type'.</t>
   </si>
 </sst>
 </file>
@@ -1950,6 +1999,262 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Hoja6"/>
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="87.5703125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja7"/>
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -2111,7 +2416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja8"/>
   <dimension ref="A1:C29"/>
@@ -2322,7 +2627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja10"/>
   <dimension ref="A1:C29"/>
@@ -2469,7 +2774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -2615,7 +2920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja9"/>
   <dimension ref="A1:C29"/>
@@ -2762,7 +3067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja11"/>
   <dimension ref="A1:C29"/>
@@ -2880,7 +3185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja12"/>
   <dimension ref="A1:C36"/>
@@ -3256,7 +3561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja13"/>
   <dimension ref="A1:C29"/>
@@ -3410,7 +3715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja14"/>
   <dimension ref="A1:C29"/>
@@ -3556,214 +3861,6 @@
       <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="B29" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Hoja15"/>
-  <dimension ref="A1:C29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="87.5703125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:3">
       <c r="B29" s="5"/>
     </row>
   </sheetData>
@@ -3965,6 +4062,214 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Hoja15"/>
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="87.5703125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja16"/>
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -4131,7 +4436,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja18"/>
   <dimension ref="A1:C29"/>
@@ -4307,7 +4612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja19"/>
   <dimension ref="A1:C26"/>
@@ -4458,7 +4763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja17"/>
   <dimension ref="A1:C29"/>
@@ -4621,7 +4926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -4783,7 +5088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -4923,7 +5228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -5061,7 +5366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C26"/>
   <sheetViews>
@@ -5258,7 +5563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -5370,170 +5675,6 @@
       </c>
       <c r="C9" s="9" t="s">
         <v>375</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" s="3" customFormat="1">
-      <c r="A11"/>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" s="3" customFormat="1">
-      <c r="A12"/>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" s="3" customFormat="1">
-      <c r="A13" s="1"/>
-      <c r="B13"/>
-    </row>
-    <row r="16" spans="1:3" s="3" customFormat="1">
-      <c r="A16" s="1"/>
-      <c r="B16"/>
-    </row>
-    <row r="18" spans="1:2" s="3" customFormat="1">
-      <c r="A18"/>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" s="3" customFormat="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" s="3" customFormat="1">
-      <c r="A20"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" s="3" customFormat="1">
-      <c r="A21"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" s="3" customFormat="1">
-      <c r="A22" s="1"/>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" s="3" customFormat="1">
-      <c r="A23"/>
-      <c r="B23" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="87.5703125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30">
-      <c r="A2" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>382</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>383</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>384</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>385</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="11" t="s">
-        <v>380</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -5819,6 +5960,170 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="87.5703125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30">
+      <c r="A2" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" s="3" customFormat="1">
+      <c r="A11"/>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" s="3" customFormat="1">
+      <c r="A12"/>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" s="3" customFormat="1">
+      <c r="A13" s="1"/>
+      <c r="B13"/>
+    </row>
+    <row r="16" spans="1:3" s="3" customFormat="1">
+      <c r="A16" s="1"/>
+      <c r="B16"/>
+    </row>
+    <row r="18" spans="1:2" s="3" customFormat="1">
+      <c r="A18"/>
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2" s="3" customFormat="1">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:2" s="3" customFormat="1">
+      <c r="A20"/>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:2" s="3" customFormat="1">
+      <c r="A21"/>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:2" s="3" customFormat="1">
+      <c r="A22" s="1"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:2" s="3" customFormat="1">
+      <c r="A23"/>
+      <c r="B23" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C29"/>
@@ -5993,7 +6298,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6242,7 +6547,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6268,7 +6573,7 @@
         <v>125</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>33</v>
+        <v>394</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>253</v>
@@ -6384,6 +6689,188 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="87.5703125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30">
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="B29" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:C29"/>
@@ -6656,7 +7143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:C29"/>
@@ -6910,260 +7397,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Hoja6"/>
-  <dimension ref="A1:C29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="87.5703125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="B29" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>